<commit_message>
create another simulation scenario
</commit_message>
<xml_diff>
--- a/simulation_results_glmm/March27_design5_ludtkesbias_contextual_estclustermeans/summary-results-bias.xlsx
+++ b/simulation_results_glmm/March27_design5_ludtkesbias_contextual_estclustermeans/summary-results-bias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\warde\Documents\GitHub\Master-Thesis\simulation_results_glmm\March27_design5_ludtkesbias_contextual_estclustermeans\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E3613AEF-D5A9-45BF-B3C5-EDD2B06BDA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52B7AA22-D45D-4215-A9A3-8583DAF5D00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1BB1EE64-70D5-44DA-9CC3-D58BF0077FAA}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1BB1EE64-70D5-44DA-9CC3-D58BF0077FAA}"/>
   </bookViews>
   <sheets>
     <sheet name="summary-results-bias" sheetId="1" r:id="rId1"/>
@@ -1029,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A87C73-ED84-43A0-B86A-CFB6D1CD22AB}">
   <dimension ref="A1:AG161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V13" sqref="V13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9974,9 +9974,6 @@
         <v>0</v>
       </c>
       <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89">
         <v>0</v>
       </c>
       <c r="I89">

</xml_diff>